<commit_message>
Did a test on an alternative method of printing the movies
</commit_message>
<xml_diff>
--- a/MovieMover/MovieList.xlsx
+++ b/MovieMover/MovieList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nat Anderson\source\repos\MovieMover\MovieMover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB7E014-5F44-454C-9193-77C1287BC6F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F4D26E-88E8-407E-86D0-40ED9829EC6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{164565E4-BE1B-4B39-A76A-EC8FDE533B3A}"/>
+    <workbookView xWindow="1098" yWindow="1098" windowWidth="17280" windowHeight="8994" xr2:uid="{164565E4-BE1B-4B39-A76A-EC8FDE533B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Latham" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="459">
   <si>
     <t>Title</t>
   </si>
@@ -1413,6 +1413,9 @@
   </si>
   <si>
     <t>Avengers: EndGame</t>
+  </si>
+  <si>
+    <t>that movie that has a super long name: someplace -  dvd - scratched - TRUE</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1496,6 +1499,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1813,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007F5DCF-4A31-4966-91D3-18D1144CDECF}">
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4900,7 +4912,9 @@
       <c r="G202" s="8"/>
     </row>
     <row r="203" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A203" s="8"/>
+      <c r="A203" s="8" t="s">
+        <v>458</v>
+      </c>
       <c r="B203" s="8"/>
       <c r="C203" s="8"/>
       <c r="D203" s="8"/>
@@ -4937,14 +4951,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCEB23C-DC0D-4B3A-A365-426357558819}">
   <dimension ref="A1:D247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="F251" sqref="F251"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="48.578125" customWidth="1"/>
-    <col min="2" max="4" width="14.578125" customWidth="1"/>
+    <col min="2" max="3" width="14.578125" customWidth="1"/>
+    <col min="4" max="4" width="14.578125" style="12" customWidth="1"/>
     <col min="5" max="5" width="10.578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4958,7 +4973,7 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4970,7 +4985,7 @@
         <v>444</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" t="b">
+      <c r="D2" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4982,7 +4997,7 @@
         <v>208</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" t="b">
+      <c r="D3" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4994,7 +5009,7 @@
         <v>208</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" t="b">
+      <c r="D4" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5006,7 +5021,7 @@
         <v>208</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" t="b">
+      <c r="D5" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5045,7 +5060,7 @@
         <v>208</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" t="b">
+      <c r="D9" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5192,7 +5207,7 @@
         <v>210</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" t="b">
+      <c r="D25" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5258,7 +5273,7 @@
         <v>210</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" t="b">
+      <c r="D32" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5270,7 +5285,7 @@
         <v>210</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" t="b">
+      <c r="D33" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5282,7 +5297,7 @@
         <v>210</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" t="b">
+      <c r="D34" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5312,7 +5327,7 @@
         <v>210</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" t="b">
+      <c r="D37" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5369,7 +5384,7 @@
         <v>210</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="3"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
@@ -5658,7 +5673,7 @@
         <v>210</v>
       </c>
       <c r="C75" s="1"/>
-      <c r="D75" t="b">
+      <c r="D75" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5724,7 +5739,7 @@
         <v>210</v>
       </c>
       <c r="C82" s="1"/>
-      <c r="D82" t="b">
+      <c r="D82" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5745,7 +5760,7 @@
         <v>210</v>
       </c>
       <c r="C84" s="1"/>
-      <c r="D84" t="b">
+      <c r="D84" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5766,7 +5781,7 @@
         <v>445</v>
       </c>
       <c r="C86" s="1"/>
-      <c r="D86" t="b">
+      <c r="D86" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5796,7 +5811,7 @@
         <v>210</v>
       </c>
       <c r="C89" s="1"/>
-      <c r="D89" t="b">
+      <c r="D89" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5990,7 +6005,7 @@
         <v>210</v>
       </c>
       <c r="C110" s="1"/>
-      <c r="D110" t="b">
+      <c r="D110" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6110,7 +6125,7 @@
         <v>210</v>
       </c>
       <c r="C123" s="1"/>
-      <c r="D123" t="b">
+      <c r="D123" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6428,7 +6443,7 @@
         <v>210</v>
       </c>
       <c r="C158" s="1"/>
-      <c r="D158" t="b">
+      <c r="D158" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6539,7 +6554,7 @@
         <v>210</v>
       </c>
       <c r="C170" s="1"/>
-      <c r="D170" t="b">
+      <c r="D170" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6758,7 +6773,7 @@
         <v>210</v>
       </c>
       <c r="C194" s="1"/>
-      <c r="D194" t="b">
+      <c r="D194" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6851,7 +6866,7 @@
         <v>210</v>
       </c>
       <c r="C204" s="1"/>
-      <c r="D204" s="2" t="b">
+      <c r="D204" s="14" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6872,7 +6887,7 @@
         <v>211</v>
       </c>
       <c r="C206" s="1"/>
-      <c r="D206" t="b">
+      <c r="D206" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6884,7 +6899,7 @@
         <v>211</v>
       </c>
       <c r="C207" s="1"/>
-      <c r="D207" t="b">
+      <c r="D207" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6896,7 +6911,7 @@
         <v>211</v>
       </c>
       <c r="C208" s="1"/>
-      <c r="D208" t="b">
+      <c r="D208" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6917,7 +6932,7 @@
         <v>211</v>
       </c>
       <c r="C210" s="1"/>
-      <c r="D210" t="b">
+      <c r="D210" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6929,7 +6944,7 @@
         <v>211</v>
       </c>
       <c r="C211" s="1"/>
-      <c r="D211" t="b">
+      <c r="D211" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6941,7 +6956,7 @@
         <v>211</v>
       </c>
       <c r="C212" s="1"/>
-      <c r="D212" t="b">
+      <c r="D212" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6971,7 +6986,7 @@
         <v>211</v>
       </c>
       <c r="C215" s="1"/>
-      <c r="D215" t="b">
+      <c r="D215" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7272,7 +7287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E6154C-948A-48FC-8F24-B9A2DB39F355}">
   <dimension ref="A1:A71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Did more tests to help solve the fornatting issues. Also separated all the printing from the sheet into their own separate methods.
</commit_message>
<xml_diff>
--- a/MovieMover/MovieList.xlsx
+++ b/MovieMover/MovieList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nat Anderson\source\repos\MovieMover\MovieMover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F4D26E-88E8-407E-86D0-40ED9829EC6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6002D96-2F17-4755-9B40-C2C1F2FBD279}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1098" yWindow="1098" windowWidth="17280" windowHeight="8994" xr2:uid="{164565E4-BE1B-4B39-A76A-EC8FDE533B3A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{164565E4-BE1B-4B39-A76A-EC8FDE533B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Latham" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="458">
   <si>
     <t>Title</t>
   </si>
@@ -1413,9 +1413,6 @@
   </si>
   <si>
     <t>Avengers: EndGame</t>
-  </si>
-  <si>
-    <t>that movie that has a super long name: someplace -  dvd - scratched - TRUE</t>
   </si>
 </sst>
 </file>
@@ -1825,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007F5DCF-4A31-4966-91D3-18D1144CDECF}">
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="A203" sqref="A203"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4912,9 +4909,7 @@
       <c r="G202" s="8"/>
     </row>
     <row r="203" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A203" s="8" t="s">
-        <v>458</v>
-      </c>
+      <c r="A203" s="8"/>
       <c r="B203" s="8"/>
       <c r="C203" s="8"/>
       <c r="D203" s="8"/>
@@ -4951,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCEB23C-DC0D-4B3A-A365-426357558819}">
   <dimension ref="A1:D247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I247"/>
+    <sheetView topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>